<commit_message>
Fix checkout: DB-only (no Excel) + keep mp.initPoint response
</commit_message>
<xml_diff>
--- a/data/cards.xlsx
+++ b/data/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berni\Desktop\coleccion-tarjetas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9715DBB-5C71-4BCE-A268-DCA63F7B3C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490F40C2-47E2-4A9F-8002-68745B8E3C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40005" yWindow="2670" windowWidth="24690" windowHeight="15345" xr2:uid="{5A110E44-25D7-4ED3-A795-D10E7F39A1FE}"/>
   </bookViews>
@@ -530,7 +530,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -601,7 +601,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -627,7 +627,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -653,7 +653,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -679,7 +679,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -708,7 +708,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
@@ -734,7 +734,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -763,7 +763,7 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
@@ -789,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -818,7 +818,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
@@ -844,7 +844,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Fix header responsive + filters mobile + PayPal + MercadoPago
</commit_message>
<xml_diff>
--- a/data/cards.xlsx
+++ b/data/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berni\Desktop\coleccion-tarjetas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53121473-A89C-4560-B153-E9BB1EF14956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA927236-C05F-4A93-BF37-D6F754975F27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47745" yWindow="1230" windowWidth="24690" windowHeight="15345" xr2:uid="{5A110E44-25D7-4ED3-A795-D10E7F39A1FE}"/>
   </bookViews>
@@ -620,7 +620,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -915,7 +915,7 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
@@ -1008,7 +1008,7 @@
         <v>12</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
@@ -1037,7 +1037,7 @@
         <v>13</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
@@ -1066,7 +1066,7 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
@@ -1095,7 +1095,7 @@
         <v>15</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -1127,7 +1127,7 @@
         <v>16</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Add pinch zoom and pan limits
</commit_message>
<xml_diff>
--- a/data/cards.xlsx
+++ b/data/cards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berni\Desktop\coleccion-tarjetas\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{553A5D1B-E42C-4901-BA7C-CD79B2B5D57F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2651AECB-AD57-4656-AE4E-1AE220F42264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="47025" yWindow="0" windowWidth="26955" windowHeight="18840" xr2:uid="{5A110E44-25D7-4ED3-A795-D10E7F39A1FE}"/>
   </bookViews>
@@ -2537,7 +2537,7 @@
   <dimension ref="A1:N338"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
-      <selection activeCell="E258" sqref="E258"/>
+      <selection activeCell="D324" sqref="D324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>